<commit_message>
Update PARTIDAS PRESUPUESTO 2024.xlsx
</commit_message>
<xml_diff>
--- a/TIC MUNICIPALIDAD PALACIO/PARTIDAS PRESUPUESTO 2024.xlsx
+++ b/TIC MUNICIPALIDAD PALACIO/PARTIDAS PRESUPUESTO 2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositorio\TIC MUNI\TIC-PALACIO\TIC MUNICIPALIDAD PALACIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECF2D0F-179C-47E6-954E-90F1480144FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4003515C-ADCF-44FC-9702-15645E554CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="434" xr2:uid="{0859E5E4-26D7-41A9-B98D-A4223A5A41B6}"/>
   </bookViews>
@@ -2973,6 +2973,36 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="13" fillId="22" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="13" fillId="22" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3004,36 +3034,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="13" fillId="11" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="13" fillId="22" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="13" fillId="22" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3409,8 +3409,8 @@
   </sheetPr>
   <dimension ref="A1:AL356"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="Q1" zoomScale="85" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="AI42" sqref="AI42:AJ45"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A60" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="AA124" sqref="AA124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3481,22 +3481,22 @@
       <c r="AK1" s="102"/>
     </row>
     <row r="2" spans="1:37" s="63" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="253" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="253" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="254" t="s">
+      <c r="B2" s="242" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="242" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="243" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="253" t="s">
+      <c r="E2" s="242" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="255" t="s">
+      <c r="F2" s="244" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="256" t="s">
+      <c r="G2" s="245" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="7"/>
@@ -3510,93 +3510,93 @@
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
       <c r="P2" s="10"/>
-      <c r="Q2" s="248" t="s">
+      <c r="Q2" s="237" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="248"/>
-      <c r="S2" s="248"/>
+      <c r="R2" s="237"/>
+      <c r="S2" s="237"/>
       <c r="T2" s="2"/>
       <c r="U2" s="4"/>
-      <c r="V2" s="236" t="s">
+      <c r="V2" s="246" t="s">
         <v>569</v>
       </c>
-      <c r="W2" s="236"/>
-      <c r="X2" s="237"/>
-      <c r="Y2" s="244" t="s">
+      <c r="W2" s="246"/>
+      <c r="X2" s="247"/>
+      <c r="Y2" s="254" t="s">
         <v>561</v>
       </c>
-      <c r="Z2" s="244"/>
-      <c r="AA2" s="244"/>
-      <c r="AB2" s="242" t="s">
+      <c r="Z2" s="254"/>
+      <c r="AA2" s="254"/>
+      <c r="AB2" s="252" t="s">
         <v>555</v>
       </c>
-      <c r="AC2" s="243"/>
-      <c r="AD2" s="243"/>
-      <c r="AE2" s="245" t="s">
+      <c r="AC2" s="253"/>
+      <c r="AD2" s="253"/>
+      <c r="AE2" s="255" t="s">
         <v>570</v>
       </c>
-      <c r="AF2" s="238" t="s">
+      <c r="AF2" s="248" t="s">
         <v>563</v>
       </c>
-      <c r="AG2" s="238"/>
-      <c r="AH2" s="239"/>
-      <c r="AI2" s="240" t="s">
+      <c r="AG2" s="248"/>
+      <c r="AH2" s="249"/>
+      <c r="AI2" s="250" t="s">
         <v>566</v>
       </c>
-      <c r="AJ2" s="240"/>
-      <c r="AK2" s="241"/>
+      <c r="AJ2" s="250"/>
+      <c r="AK2" s="251"/>
     </row>
     <row r="3" spans="1:37" s="63" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="253"/>
-      <c r="C3" s="253"/>
-      <c r="D3" s="254"/>
-      <c r="E3" s="253"/>
-      <c r="F3" s="255"/>
-      <c r="G3" s="256"/>
-      <c r="H3" s="249" t="s">
+      <c r="B3" s="242"/>
+      <c r="C3" s="242"/>
+      <c r="D3" s="243"/>
+      <c r="E3" s="242"/>
+      <c r="F3" s="244"/>
+      <c r="G3" s="245"/>
+      <c r="H3" s="238" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="250"/>
-      <c r="J3" s="251"/>
-      <c r="K3" s="252" t="s">
+      <c r="I3" s="239"/>
+      <c r="J3" s="240"/>
+      <c r="K3" s="241" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="252"/>
-      <c r="M3" s="252"/>
-      <c r="N3" s="252" t="s">
+      <c r="L3" s="241"/>
+      <c r="M3" s="241"/>
+      <c r="N3" s="241" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="252"/>
-      <c r="P3" s="252"/>
-      <c r="Q3" s="248"/>
-      <c r="R3" s="248"/>
-      <c r="S3" s="248"/>
+      <c r="O3" s="241"/>
+      <c r="P3" s="241"/>
+      <c r="Q3" s="237"/>
+      <c r="R3" s="237"/>
+      <c r="S3" s="237"/>
       <c r="T3" s="2"/>
       <c r="U3" s="4"/>
-      <c r="V3" s="236"/>
-      <c r="W3" s="236"/>
-      <c r="X3" s="237"/>
-      <c r="Y3" s="244"/>
-      <c r="Z3" s="244"/>
-      <c r="AA3" s="244"/>
-      <c r="AB3" s="242"/>
-      <c r="AC3" s="243"/>
-      <c r="AD3" s="243"/>
-      <c r="AE3" s="246"/>
-      <c r="AF3" s="238"/>
-      <c r="AG3" s="238"/>
-      <c r="AH3" s="239"/>
-      <c r="AI3" s="240"/>
-      <c r="AJ3" s="240"/>
-      <c r="AK3" s="241"/>
+      <c r="V3" s="246"/>
+      <c r="W3" s="246"/>
+      <c r="X3" s="247"/>
+      <c r="Y3" s="254"/>
+      <c r="Z3" s="254"/>
+      <c r="AA3" s="254"/>
+      <c r="AB3" s="252"/>
+      <c r="AC3" s="253"/>
+      <c r="AD3" s="253"/>
+      <c r="AE3" s="256"/>
+      <c r="AF3" s="248"/>
+      <c r="AG3" s="248"/>
+      <c r="AH3" s="249"/>
+      <c r="AI3" s="250"/>
+      <c r="AJ3" s="250"/>
+      <c r="AK3" s="251"/>
     </row>
     <row r="4" spans="1:37" s="63" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="253"/>
-      <c r="C4" s="253"/>
-      <c r="D4" s="254"/>
-      <c r="E4" s="253"/>
-      <c r="F4" s="255"/>
-      <c r="G4" s="256"/>
+      <c r="B4" s="242"/>
+      <c r="C4" s="242"/>
+      <c r="D4" s="243"/>
+      <c r="E4" s="242"/>
+      <c r="F4" s="244"/>
+      <c r="G4" s="245"/>
       <c r="H4" s="11" t="s">
         <v>11</v>
       </c>
@@ -3818,7 +3818,7 @@
       <c r="AJ7" s="216"/>
       <c r="AK7" s="216"/>
     </row>
-    <row r="8" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="80" t="s">
         <v>555</v>
       </c>
@@ -3914,7 +3914,7 @@
       <c r="AJ8" s="216"/>
       <c r="AK8" s="216"/>
     </row>
-    <row r="9" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="80" t="s">
         <v>555</v>
       </c>
@@ -4010,7 +4010,7 @@
       <c r="AJ9" s="216"/>
       <c r="AK9" s="216"/>
     </row>
-    <row r="10" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="80" t="s">
         <v>555</v>
       </c>
@@ -4106,7 +4106,7 @@
       <c r="AJ10" s="216"/>
       <c r="AK10" s="216"/>
     </row>
-    <row r="11" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="80" t="s">
         <v>555</v>
       </c>
@@ -4202,7 +4202,7 @@
       <c r="AJ11" s="216"/>
       <c r="AK11" s="216"/>
     </row>
-    <row r="12" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="80" t="s">
         <v>562</v>
       </c>
@@ -4275,9 +4275,16 @@
       <c r="V12" s="114"/>
       <c r="W12" s="114"/>
       <c r="X12" s="114"/>
-      <c r="Y12" s="201"/>
-      <c r="Z12" s="206"/>
-      <c r="AA12" s="206"/>
+      <c r="Y12" s="201">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="206">
+        <v>3950.21</v>
+      </c>
+      <c r="AA12" s="206">
+        <f>Y12*Z12</f>
+        <v>3950.21</v>
+      </c>
       <c r="AB12" s="210">
         <v>1</v>
       </c>
@@ -4394,7 +4401,7 @@
       <c r="AJ14" s="216"/>
       <c r="AK14" s="216"/>
     </row>
-    <row r="15" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="80" t="s">
         <v>567</v>
       </c>
@@ -4490,7 +4497,7 @@
       <c r="AJ15" s="216"/>
       <c r="AK15" s="216"/>
     </row>
-    <row r="16" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="80" t="s">
         <v>567</v>
       </c>
@@ -4634,7 +4641,7 @@
       <c r="AJ17" s="216"/>
       <c r="AK17" s="216"/>
     </row>
-    <row r="18" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="80" t="s">
         <v>573</v>
       </c>
@@ -4721,7 +4728,7 @@
       <c r="AJ18" s="216"/>
       <c r="AK18" s="216"/>
     </row>
-    <row r="19" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="80" t="s">
         <v>573</v>
       </c>
@@ -4808,7 +4815,7 @@
       <c r="AJ19" s="216"/>
       <c r="AK19" s="216"/>
     </row>
-    <row r="20" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="80" t="s">
         <v>573</v>
       </c>
@@ -5870,7 +5877,7 @@
       <c r="AJ33" s="216"/>
       <c r="AK33" s="216"/>
     </row>
-    <row r="34" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="80" t="s">
         <v>573</v>
       </c>
@@ -5957,7 +5964,7 @@
       <c r="AJ34" s="216"/>
       <c r="AK34" s="216"/>
     </row>
-    <row r="35" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="80" t="s">
         <v>573</v>
       </c>
@@ -6044,7 +6051,7 @@
       <c r="AJ35" s="216"/>
       <c r="AK35" s="216"/>
     </row>
-    <row r="36" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="80" t="s">
         <v>573</v>
       </c>
@@ -6131,7 +6138,7 @@
       <c r="AJ36" s="216"/>
       <c r="AK36" s="216"/>
     </row>
-    <row r="37" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="80" t="s">
         <v>573</v>
       </c>
@@ -6266,7 +6273,7 @@
       <c r="AJ38" s="216"/>
       <c r="AK38" s="216"/>
     </row>
-    <row r="39" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="80" t="s">
         <v>555</v>
       </c>
@@ -6353,7 +6360,7 @@
       <c r="AJ39" s="216"/>
       <c r="AK39" s="216"/>
     </row>
-    <row r="40" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="80" t="s">
         <v>573</v>
       </c>
@@ -6443,7 +6450,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="80" t="s">
         <v>574</v>
       </c>
@@ -6721,7 +6728,7 @@
         <v>7280</v>
       </c>
     </row>
-    <row r="44" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="80" t="s">
         <v>573</v>
       </c>
@@ -6905,7 +6912,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="80" t="s">
         <v>562</v>
       </c>
@@ -6999,7 +7006,7 @@
       <c r="AJ46" s="216"/>
       <c r="AK46" s="216"/>
     </row>
-    <row r="47" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="80" t="s">
         <v>562</v>
       </c>
@@ -7350,7 +7357,7 @@
       <c r="AJ52" s="216"/>
       <c r="AK52" s="216"/>
     </row>
-    <row r="53" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="80" t="s">
         <v>562</v>
       </c>
@@ -7540,7 +7547,7 @@
       <c r="AJ55" s="216"/>
       <c r="AK55" s="216"/>
     </row>
-    <row r="56" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="80" t="s">
         <v>567</v>
       </c>
@@ -7684,7 +7691,7 @@
       <c r="AJ57" s="216"/>
       <c r="AK57" s="216"/>
     </row>
-    <row r="58" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="80" t="s">
         <v>573</v>
       </c>
@@ -7771,7 +7778,7 @@
       <c r="AJ58" s="216"/>
       <c r="AK58" s="216"/>
     </row>
-    <row r="59" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="80" t="s">
         <v>573</v>
       </c>
@@ -7858,7 +7865,7 @@
       <c r="AJ59" s="216"/>
       <c r="AK59" s="216"/>
     </row>
-    <row r="60" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="80" t="s">
         <v>573</v>
       </c>
@@ -8872,7 +8879,7 @@
       <c r="AJ72" s="216"/>
       <c r="AK72" s="216"/>
     </row>
-    <row r="73" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="80" t="s">
         <v>573</v>
       </c>
@@ -9007,7 +9014,7 @@
       <c r="AJ74" s="216"/>
       <c r="AK74" s="216"/>
     </row>
-    <row r="75" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="80" t="s">
         <v>573</v>
       </c>
@@ -9094,7 +9101,7 @@
       <c r="AJ75" s="216"/>
       <c r="AK75" s="216"/>
     </row>
-    <row r="76" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="80" t="s">
         <v>573</v>
       </c>
@@ -9181,7 +9188,7 @@
       <c r="AJ76" s="216"/>
       <c r="AK76" s="216"/>
     </row>
-    <row r="77" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="80" t="s">
         <v>573</v>
       </c>
@@ -9268,7 +9275,7 @@
       <c r="AJ77" s="216"/>
       <c r="AK77" s="216"/>
     </row>
-    <row r="78" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="80" t="s">
         <v>573</v>
       </c>
@@ -9355,7 +9362,7 @@
       <c r="AJ78" s="216"/>
       <c r="AK78" s="216"/>
     </row>
-    <row r="79" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="80" t="s">
         <v>573</v>
       </c>
@@ -9500,16 +9507,16 @@
       <c r="C81" s="81" t="s">
         <v>146</v>
       </c>
-      <c r="D81" s="23" t="s">
+      <c r="D81" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="E81" s="24">
+      <c r="E81" s="83">
         <v>2</v>
       </c>
-      <c r="F81" s="25">
+      <c r="F81" s="84">
         <v>34.22</v>
       </c>
-      <c r="G81" s="53">
+      <c r="G81" s="85">
         <f t="shared" si="11"/>
         <v>68.44</v>
       </c>
@@ -9625,7 +9632,7 @@
       <c r="AJ82" s="216"/>
       <c r="AK82" s="216"/>
     </row>
-    <row r="83" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="80" t="s">
         <v>573</v>
       </c>
@@ -9808,7 +9815,7 @@
       <c r="AJ85" s="216"/>
       <c r="AK85" s="216"/>
     </row>
-    <row r="86" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="80" t="s">
         <v>567</v>
       </c>
@@ -9903,7 +9910,7 @@
       <c r="AJ86" s="216"/>
       <c r="AK86" s="216"/>
     </row>
-    <row r="87" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="80" t="s">
         <v>567</v>
       </c>
@@ -10046,7 +10053,7 @@
       <c r="AJ88" s="216"/>
       <c r="AK88" s="216"/>
     </row>
-    <row r="89" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="80" t="s">
         <v>573</v>
       </c>
@@ -10133,7 +10140,7 @@
       <c r="AJ89" s="216"/>
       <c r="AK89" s="216"/>
     </row>
-    <row r="90" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="80" t="s">
         <v>573</v>
       </c>
@@ -10220,7 +10227,7 @@
       <c r="AJ90" s="216"/>
       <c r="AK90" s="216"/>
     </row>
-    <row r="91" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="80" t="s">
         <v>573</v>
       </c>
@@ -10307,7 +10314,7 @@
       <c r="AJ91" s="216"/>
       <c r="AK91" s="216"/>
     </row>
-    <row r="92" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="80" t="s">
         <v>573</v>
       </c>
@@ -10394,7 +10401,7 @@
       <c r="AJ92" s="216"/>
       <c r="AK92" s="216"/>
     </row>
-    <row r="93" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="80" t="s">
         <v>573</v>
       </c>
@@ -11636,7 +11643,7 @@
       <c r="AJ108" s="216"/>
       <c r="AK108" s="216"/>
     </row>
-    <row r="109" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="80" t="s">
         <v>573</v>
       </c>
@@ -11771,7 +11778,7 @@
       <c r="AJ110" s="216"/>
       <c r="AK110" s="216"/>
     </row>
-    <row r="111" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="80" t="s">
         <v>573</v>
       </c>
@@ -11906,7 +11913,7 @@
       <c r="AJ112" s="216"/>
       <c r="AK112" s="216"/>
     </row>
-    <row r="113" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="80" t="s">
         <v>573</v>
       </c>
@@ -11993,7 +12000,7 @@
       <c r="AJ113" s="216"/>
       <c r="AK113" s="216"/>
     </row>
-    <row r="114" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="80" t="s">
         <v>573</v>
       </c>
@@ -12080,7 +12087,7 @@
       <c r="AJ114" s="216"/>
       <c r="AK114" s="216"/>
     </row>
-    <row r="115" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="80" t="s">
         <v>573</v>
       </c>
@@ -12167,7 +12174,7 @@
       <c r="AJ115" s="216"/>
       <c r="AK115" s="216"/>
     </row>
-    <row r="116" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="80" t="s">
         <v>573</v>
       </c>
@@ -12254,7 +12261,7 @@
       <c r="AJ116" s="216"/>
       <c r="AK116" s="216"/>
     </row>
-    <row r="117" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="80" t="s">
         <v>573</v>
       </c>
@@ -12341,7 +12348,7 @@
       <c r="AJ117" s="216"/>
       <c r="AK117" s="216"/>
     </row>
-    <row r="118" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="80" t="s">
         <v>573</v>
       </c>
@@ -12428,7 +12435,7 @@
       <c r="AJ118" s="216"/>
       <c r="AK118" s="216"/>
     </row>
-    <row r="119" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="80" t="s">
         <v>573</v>
       </c>
@@ -12515,7 +12522,7 @@
       <c r="AJ119" s="216"/>
       <c r="AK119" s="216"/>
     </row>
-    <row r="120" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="80" t="s">
         <v>573</v>
       </c>
@@ -12650,9 +12657,9 @@
       <c r="AJ121" s="216"/>
       <c r="AK121" s="216"/>
     </row>
-    <row r="122" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="80" t="s">
-        <v>573</v>
+        <v>562</v>
       </c>
       <c r="B122" s="81" t="s">
         <v>215</v>
@@ -12723,9 +12730,16 @@
       <c r="V122" s="114"/>
       <c r="W122" s="114"/>
       <c r="X122" s="114"/>
-      <c r="Y122" s="201"/>
-      <c r="Z122" s="206"/>
-      <c r="AA122" s="206"/>
+      <c r="Y122" s="201">
+        <v>209</v>
+      </c>
+      <c r="Z122" s="206">
+        <v>84.75</v>
+      </c>
+      <c r="AA122" s="206">
+        <f>Y122*Z122</f>
+        <v>17712.75</v>
+      </c>
       <c r="AB122" s="210"/>
       <c r="AC122" s="211"/>
       <c r="AD122" s="211"/>
@@ -12785,7 +12799,7 @@
       <c r="AJ123" s="216"/>
       <c r="AK123" s="216"/>
     </row>
-    <row r="124" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="80" t="s">
         <v>567</v>
       </c>
@@ -12881,7 +12895,7 @@
       <c r="AJ124" s="216"/>
       <c r="AK124" s="216"/>
     </row>
-    <row r="125" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="80" t="s">
         <v>567</v>
       </c>
@@ -13025,7 +13039,7 @@
       <c r="AJ126" s="216"/>
       <c r="AK126" s="216"/>
     </row>
-    <row r="127" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="80" t="s">
         <v>573</v>
       </c>
@@ -13112,7 +13126,7 @@
       <c r="AJ127" s="216"/>
       <c r="AK127" s="216"/>
     </row>
-    <row r="128" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="80" t="s">
         <v>567</v>
       </c>
@@ -13207,7 +13221,7 @@
       <c r="AJ128" s="216"/>
       <c r="AK128" s="216"/>
     </row>
-    <row r="129" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="80" t="s">
         <v>567</v>
       </c>
@@ -13302,7 +13316,7 @@
       <c r="AJ129" s="216"/>
       <c r="AK129" s="216"/>
     </row>
-    <row r="130" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="80" t="s">
         <v>567</v>
       </c>
@@ -13397,7 +13411,7 @@
       <c r="AJ130" s="216"/>
       <c r="AK130" s="216"/>
     </row>
-    <row r="131" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="80" t="s">
         <v>573</v>
       </c>
@@ -13484,7 +13498,7 @@
       <c r="AJ131" s="216"/>
       <c r="AK131" s="216"/>
     </row>
-    <row r="132" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="80" t="s">
         <v>555</v>
       </c>
@@ -13571,7 +13585,7 @@
       <c r="AJ132" s="216"/>
       <c r="AK132" s="216"/>
     </row>
-    <row r="133" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="80" t="s">
         <v>562</v>
       </c>
@@ -13857,7 +13871,7 @@
       <c r="AJ137" s="216"/>
       <c r="AK137" s="216"/>
     </row>
-    <row r="138" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="80" t="s">
         <v>573</v>
       </c>
@@ -13947,7 +13961,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="139" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="80" t="s">
         <v>573</v>
       </c>
@@ -14085,7 +14099,7 @@
       <c r="AJ140" s="216"/>
       <c r="AK140" s="216"/>
     </row>
-    <row r="141" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="80" t="s">
         <v>573</v>
       </c>
@@ -14223,7 +14237,7 @@
       <c r="AJ142" s="216"/>
       <c r="AK142" s="216"/>
     </row>
-    <row r="143" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="80" t="s">
         <v>567</v>
       </c>
@@ -14319,7 +14333,7 @@
       <c r="AJ143" s="216"/>
       <c r="AK143" s="216"/>
     </row>
-    <row r="144" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="80" t="s">
         <v>567</v>
       </c>
@@ -14415,7 +14429,7 @@
       <c r="AJ144" s="216"/>
       <c r="AK144" s="216"/>
     </row>
-    <row r="145" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="80" t="s">
         <v>567</v>
       </c>
@@ -14511,7 +14525,7 @@
       <c r="AJ145" s="216"/>
       <c r="AK145" s="216"/>
     </row>
-    <row r="146" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="80" t="s">
         <v>573</v>
       </c>
@@ -14598,7 +14612,7 @@
       <c r="AJ146" s="216"/>
       <c r="AK146" s="216"/>
     </row>
-    <row r="147" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="80" t="s">
         <v>573</v>
       </c>
@@ -14685,7 +14699,7 @@
       <c r="AJ147" s="216"/>
       <c r="AK147" s="216"/>
     </row>
-    <row r="148" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="80" t="s">
         <v>573</v>
       </c>
@@ -14868,7 +14882,7 @@
       <c r="AJ150" s="216"/>
       <c r="AK150" s="216"/>
     </row>
-    <row r="151" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="80" t="s">
         <v>573</v>
       </c>
@@ -14955,7 +14969,7 @@
       <c r="AJ151" s="216"/>
       <c r="AK151" s="216"/>
     </row>
-    <row r="152" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="80" t="s">
         <v>567</v>
       </c>
@@ -15099,7 +15113,7 @@
       <c r="AJ153" s="216"/>
       <c r="AK153" s="216"/>
     </row>
-    <row r="154" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="80" t="s">
         <v>573</v>
       </c>
@@ -15273,7 +15287,7 @@
       <c r="AJ155" s="216"/>
       <c r="AK155" s="216"/>
     </row>
-    <row r="156" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="80" t="s">
         <v>573</v>
       </c>
@@ -15360,7 +15374,7 @@
       <c r="AJ156" s="216"/>
       <c r="AK156" s="216"/>
     </row>
-    <row r="157" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="80" t="s">
         <v>573</v>
       </c>
@@ -15447,7 +15461,7 @@
       <c r="AJ157" s="216"/>
       <c r="AK157" s="216"/>
     </row>
-    <row r="158" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="80" t="s">
         <v>573</v>
       </c>
@@ -15621,7 +15635,7 @@
       <c r="AJ159" s="216"/>
       <c r="AK159" s="216"/>
     </row>
-    <row r="160" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="80" t="s">
         <v>573</v>
       </c>
@@ -15795,7 +15809,7 @@
       <c r="AJ161" s="216"/>
       <c r="AK161" s="216"/>
     </row>
-    <row r="162" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="80" t="s">
         <v>573</v>
       </c>
@@ -15969,7 +15983,7 @@
       <c r="AJ163" s="216"/>
       <c r="AK163" s="216"/>
     </row>
-    <row r="164" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="80" t="s">
         <v>573</v>
       </c>
@@ -16713,7 +16727,7 @@
       <c r="AJ172" s="216"/>
       <c r="AK172" s="216"/>
     </row>
-    <row r="173" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="80" t="s">
         <v>573</v>
       </c>
@@ -16848,7 +16862,7 @@
       <c r="AJ174" s="216"/>
       <c r="AK174" s="216"/>
     </row>
-    <row r="175" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="80" t="s">
         <v>573</v>
       </c>
@@ -16935,7 +16949,7 @@
       <c r="AJ175" s="216"/>
       <c r="AK175" s="216"/>
     </row>
-    <row r="176" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="80" t="s">
         <v>573</v>
       </c>
@@ -17022,7 +17036,7 @@
       <c r="AJ176" s="216"/>
       <c r="AK176" s="216"/>
     </row>
-    <row r="177" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="80" t="s">
         <v>573</v>
       </c>
@@ -17640,7 +17654,7 @@
       <c r="AJ184" s="216"/>
       <c r="AK184" s="216"/>
     </row>
-    <row r="185" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="80" t="s">
         <v>573</v>
       </c>
@@ -17730,7 +17744,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="186" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="80" t="s">
         <v>573</v>
       </c>
@@ -17868,7 +17882,7 @@
       <c r="AJ187" s="216"/>
       <c r="AK187" s="216"/>
     </row>
-    <row r="188" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="80" t="s">
         <v>567</v>
       </c>
@@ -17964,7 +17978,7 @@
       <c r="AJ188" s="216"/>
       <c r="AK188" s="216"/>
     </row>
-    <row r="189" spans="1:38" s="80" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:38" s="80" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A189" s="80" t="s">
         <v>567</v>
       </c>
@@ -18108,7 +18122,7 @@
       <c r="AJ190" s="216"/>
       <c r="AK190" s="216"/>
     </row>
-    <row r="191" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="80" t="s">
         <v>573</v>
       </c>
@@ -18195,7 +18209,7 @@
       <c r="AJ191" s="216"/>
       <c r="AK191" s="216"/>
     </row>
-    <row r="192" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="80" t="s">
         <v>573</v>
       </c>
@@ -18282,7 +18296,7 @@
       <c r="AJ192" s="216"/>
       <c r="AK192" s="216"/>
     </row>
-    <row r="193" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="80" t="s">
         <v>573</v>
       </c>
@@ -18804,7 +18818,7 @@
       <c r="AJ198" s="216"/>
       <c r="AK198" s="216"/>
     </row>
-    <row r="199" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="80" t="s">
         <v>573</v>
       </c>
@@ -18978,7 +18992,7 @@
       <c r="AJ200" s="216"/>
       <c r="AK200" s="216"/>
     </row>
-    <row r="201" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="80" t="s">
         <v>573</v>
       </c>
@@ -19065,7 +19079,7 @@
       <c r="AJ201" s="216"/>
       <c r="AK201" s="216"/>
     </row>
-    <row r="202" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="80" t="s">
         <v>573</v>
       </c>
@@ -19200,7 +19214,7 @@
       <c r="AJ203" s="216"/>
       <c r="AK203" s="216"/>
     </row>
-    <row r="204" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="80" t="s">
         <v>573</v>
       </c>
@@ -19287,7 +19301,7 @@
       <c r="AJ204" s="216"/>
       <c r="AK204" s="216"/>
     </row>
-    <row r="205" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="80" t="s">
         <v>573</v>
       </c>
@@ -19377,7 +19391,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="206" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="80" t="s">
         <v>573</v>
       </c>
@@ -19464,7 +19478,7 @@
       <c r="AJ206" s="216"/>
       <c r="AK206" s="216"/>
     </row>
-    <row r="207" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="80" t="s">
         <v>573</v>
       </c>
@@ -19551,7 +19565,7 @@
       <c r="AJ207" s="216"/>
       <c r="AK207" s="216"/>
     </row>
-    <row r="208" spans="1:38" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:38" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="80" t="s">
         <v>573</v>
       </c>
@@ -19734,7 +19748,7 @@
       <c r="AJ210" s="216"/>
       <c r="AK210" s="216"/>
     </row>
-    <row r="211" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="80" t="s">
         <v>571</v>
       </c>
@@ -19821,7 +19835,7 @@
       <c r="AJ211" s="216"/>
       <c r="AK211" s="216"/>
     </row>
-    <row r="212" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="80" t="s">
         <v>571</v>
       </c>
@@ -19908,7 +19922,7 @@
       <c r="AJ212" s="216"/>
       <c r="AK212" s="216"/>
     </row>
-    <row r="213" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="80" t="s">
         <v>571</v>
       </c>
@@ -19995,7 +20009,7 @@
       <c r="AJ213" s="216"/>
       <c r="AK213" s="216"/>
     </row>
-    <row r="214" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="80" t="s">
         <v>571</v>
       </c>
@@ -20082,7 +20096,7 @@
       <c r="AJ214" s="216"/>
       <c r="AK214" s="216"/>
     </row>
-    <row r="215" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="80" t="s">
         <v>571</v>
       </c>
@@ -20169,7 +20183,7 @@
       <c r="AJ215" s="216"/>
       <c r="AK215" s="216"/>
     </row>
-    <row r="216" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="80" t="s">
         <v>571</v>
       </c>
@@ -20256,7 +20270,7 @@
       <c r="AJ216" s="216"/>
       <c r="AK216" s="216"/>
     </row>
-    <row r="217" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="80" t="s">
         <v>571</v>
       </c>
@@ -20343,7 +20357,7 @@
       <c r="AJ217" s="216"/>
       <c r="AK217" s="216"/>
     </row>
-    <row r="218" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="80" t="s">
         <v>571</v>
       </c>
@@ -20430,7 +20444,7 @@
       <c r="AJ218" s="216"/>
       <c r="AK218" s="216"/>
     </row>
-    <row r="219" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="80" t="s">
         <v>571</v>
       </c>
@@ -20517,7 +20531,7 @@
       <c r="AJ219" s="216"/>
       <c r="AK219" s="216"/>
     </row>
-    <row r="220" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="80" t="s">
         <v>571</v>
       </c>
@@ -20652,7 +20666,7 @@
       <c r="AJ221" s="216"/>
       <c r="AK221" s="216"/>
     </row>
-    <row r="222" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="80" t="s">
         <v>571</v>
       </c>
@@ -20739,7 +20753,7 @@
       <c r="AJ222" s="216"/>
       <c r="AK222" s="216"/>
     </row>
-    <row r="223" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="80" t="s">
         <v>571</v>
       </c>
@@ -20826,7 +20840,7 @@
       <c r="AJ223" s="216"/>
       <c r="AK223" s="216"/>
     </row>
-    <row r="224" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="80" t="s">
         <v>571</v>
       </c>
@@ -20913,7 +20927,7 @@
       <c r="AJ224" s="216"/>
       <c r="AK224" s="216"/>
     </row>
-    <row r="225" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="80" t="s">
         <v>571</v>
       </c>
@@ -21000,7 +21014,7 @@
       <c r="AJ225" s="216"/>
       <c r="AK225" s="216"/>
     </row>
-    <row r="226" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="80" t="s">
         <v>571</v>
       </c>
@@ -21087,7 +21101,7 @@
       <c r="AJ226" s="216"/>
       <c r="AK226" s="216"/>
     </row>
-    <row r="227" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="80" t="s">
         <v>571</v>
       </c>
@@ -21174,7 +21188,7 @@
       <c r="AJ227" s="216"/>
       <c r="AK227" s="216"/>
     </row>
-    <row r="228" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="80" t="s">
         <v>571</v>
       </c>
@@ -21261,7 +21275,7 @@
       <c r="AJ228" s="216"/>
       <c r="AK228" s="216"/>
     </row>
-    <row r="229" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="80" t="s">
         <v>571</v>
       </c>
@@ -21348,7 +21362,7 @@
       <c r="AJ229" s="216"/>
       <c r="AK229" s="216"/>
     </row>
-    <row r="230" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="80" t="s">
         <v>571</v>
       </c>
@@ -21435,7 +21449,7 @@
       <c r="AJ230" s="216"/>
       <c r="AK230" s="216"/>
     </row>
-    <row r="231" spans="1:37" s="80" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:37" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="80" t="s">
         <v>571</v>
       </c>
@@ -22045,7 +22059,7 @@
       <c r="AJ238" s="217"/>
       <c r="AK238" s="217"/>
     </row>
-    <row r="239" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="65" t="s">
         <v>573</v>
       </c>
@@ -22130,7 +22144,7 @@
       <c r="AJ239" s="217"/>
       <c r="AK239" s="217"/>
     </row>
-    <row r="240" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="65" t="s">
         <v>573</v>
       </c>
@@ -22358,7 +22372,7 @@
       <c r="AJ242" s="217"/>
       <c r="AK242" s="217"/>
     </row>
-    <row r="243" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="65" t="s">
         <v>573</v>
       </c>
@@ -22443,7 +22457,7 @@
       <c r="AJ243" s="217"/>
       <c r="AK243" s="217"/>
     </row>
-    <row r="244" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="65" t="s">
         <v>573</v>
       </c>
@@ -23014,7 +23028,7 @@
       <c r="AJ252" s="217"/>
       <c r="AK252" s="217"/>
     </row>
-    <row r="253" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" s="65" t="s">
         <v>573</v>
       </c>
@@ -23101,7 +23115,7 @@
       <c r="AJ253" s="217"/>
       <c r="AK253" s="217"/>
     </row>
-    <row r="254" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" s="65" t="s">
         <v>573</v>
       </c>
@@ -23188,7 +23202,7 @@
       <c r="AJ254" s="217"/>
       <c r="AK254" s="217"/>
     </row>
-    <row r="255" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" s="65" t="s">
         <v>573</v>
       </c>
@@ -23761,7 +23775,7 @@
       <c r="AJ263" s="217"/>
       <c r="AK263" s="217"/>
     </row>
-    <row r="264" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A264" s="80" t="s">
         <v>571</v>
       </c>
@@ -23841,15 +23855,15 @@
         <v>2</v>
       </c>
       <c r="AC264" s="211">
-        <v>146858.42000000001</v>
+        <v>125000</v>
       </c>
       <c r="AD264" s="211">
         <f>AB264*AC264</f>
-        <v>293716.84000000003</v>
+        <v>250000</v>
       </c>
       <c r="AE264" s="211">
         <f>AD264-G264</f>
-        <v>-163743.15999999997</v>
+        <v>-207460</v>
       </c>
       <c r="AF264" s="159"/>
       <c r="AG264" s="159"/>
@@ -23858,7 +23872,7 @@
       <c r="AJ264" s="217"/>
       <c r="AK264" s="217"/>
     </row>
-    <row r="265" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A265" s="173" t="s">
         <v>562</v>
       </c>
@@ -23997,7 +24011,7 @@
       <c r="AJ266" s="217"/>
       <c r="AK266" s="217"/>
     </row>
-    <row r="267" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A267" s="65" t="s">
         <v>573</v>
       </c>
@@ -24084,7 +24098,7 @@
       <c r="AJ267" s="217"/>
       <c r="AK267" s="217"/>
     </row>
-    <row r="268" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A268" s="173" t="s">
         <v>574</v>
       </c>
@@ -24171,7 +24185,7 @@
       <c r="AJ268" s="217"/>
       <c r="AK268" s="217"/>
     </row>
-    <row r="269" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A269" s="65" t="s">
         <v>573</v>
       </c>
@@ -24258,7 +24272,7 @@
       <c r="AJ269" s="217"/>
       <c r="AK269" s="217"/>
     </row>
-    <row r="270" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A270" s="65" t="s">
         <v>573</v>
       </c>
@@ -24534,7 +24548,7 @@
       <c r="AJ273" s="217"/>
       <c r="AK273" s="217"/>
     </row>
-    <row r="274" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A274" s="173" t="s">
         <v>563</v>
       </c>
@@ -24648,7 +24662,7 @@
       <c r="AJ275" s="217"/>
       <c r="AK275" s="217"/>
     </row>
-    <row r="276" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A276" s="65" t="s">
         <v>573</v>
       </c>
@@ -24780,7 +24794,7 @@
       <c r="AJ277" s="217"/>
       <c r="AK277" s="217"/>
     </row>
-    <row r="278" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A278" s="173" t="s">
         <v>562</v>
       </c>
@@ -24874,7 +24888,7 @@
       <c r="AJ278" s="217"/>
       <c r="AK278" s="217"/>
     </row>
-    <row r="279" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A279" s="173" t="s">
         <v>562</v>
       </c>
@@ -24968,7 +24982,7 @@
       <c r="AJ279" s="217"/>
       <c r="AK279" s="217"/>
     </row>
-    <row r="280" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A280" s="173" t="s">
         <v>562</v>
       </c>
@@ -25292,7 +25306,7 @@
       <c r="AJ284" s="217"/>
       <c r="AK284" s="217"/>
     </row>
-    <row r="285" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A285" s="80" t="s">
         <v>555</v>
       </c>
@@ -25389,7 +25403,7 @@
       <c r="AJ285" s="217"/>
       <c r="AK285" s="217"/>
     </row>
-    <row r="286" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A286" s="80" t="s">
         <v>555</v>
       </c>
@@ -25924,7 +25938,7 @@
       <c r="AJ292" s="217"/>
       <c r="AK292" s="217"/>
     </row>
-    <row r="293" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A293" s="65" t="s">
         <v>573</v>
       </c>
@@ -26011,7 +26025,7 @@
       <c r="AJ293" s="217"/>
       <c r="AK293" s="217"/>
     </row>
-    <row r="294" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A294" s="65" t="s">
         <v>573</v>
       </c>
@@ -26098,7 +26112,7 @@
       <c r="AJ294" s="217"/>
       <c r="AK294" s="217"/>
     </row>
-    <row r="295" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A295" s="65" t="s">
         <v>573</v>
       </c>
@@ -26185,7 +26199,7 @@
       <c r="AJ295" s="217"/>
       <c r="AK295" s="217"/>
     </row>
-    <row r="296" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A296" s="65" t="s">
         <v>573</v>
       </c>
@@ -26272,7 +26286,7 @@
       <c r="AJ296" s="217"/>
       <c r="AK296" s="217"/>
     </row>
-    <row r="297" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A297" s="65" t="s">
         <v>573</v>
       </c>
@@ -26359,7 +26373,7 @@
       <c r="AJ297" s="217"/>
       <c r="AK297" s="217"/>
     </row>
-    <row r="298" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A298" s="65" t="s">
         <v>573</v>
       </c>
@@ -26446,7 +26460,7 @@
       <c r="AJ298" s="217"/>
       <c r="AK298" s="217"/>
     </row>
-    <row r="299" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A299" s="65" t="s">
         <v>573</v>
       </c>
@@ -26533,7 +26547,7 @@
       <c r="AJ299" s="217"/>
       <c r="AK299" s="217"/>
     </row>
-    <row r="300" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A300" s="65" t="s">
         <v>573</v>
       </c>
@@ -26620,7 +26634,7 @@
       <c r="AJ300" s="217"/>
       <c r="AK300" s="217"/>
     </row>
-    <row r="301" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A301" s="65" t="s">
         <v>573</v>
       </c>
@@ -26707,7 +26721,7 @@
       <c r="AJ301" s="217"/>
       <c r="AK301" s="217"/>
     </row>
-    <row r="302" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A302" s="65" t="s">
         <v>573</v>
       </c>
@@ -26794,7 +26808,7 @@
       <c r="AJ302" s="217"/>
       <c r="AK302" s="217"/>
     </row>
-    <row r="303" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A303" s="65" t="s">
         <v>573</v>
       </c>
@@ -26926,7 +26940,7 @@
       <c r="AJ304" s="217"/>
       <c r="AK304" s="217"/>
     </row>
-    <row r="305" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A305" s="65" t="s">
         <v>573</v>
       </c>
@@ -27013,7 +27027,7 @@
       <c r="AJ305" s="217"/>
       <c r="AK305" s="217"/>
     </row>
-    <row r="306" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A306" s="65" t="s">
         <v>573</v>
       </c>
@@ -27100,7 +27114,7 @@
       <c r="AJ306" s="217"/>
       <c r="AK306" s="217"/>
     </row>
-    <row r="307" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A307" s="65" t="s">
         <v>573</v>
       </c>
@@ -27187,7 +27201,7 @@
       <c r="AJ307" s="217"/>
       <c r="AK307" s="217"/>
     </row>
-    <row r="308" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A308" s="65" t="s">
         <v>573</v>
       </c>
@@ -27274,7 +27288,7 @@
       <c r="AJ308" s="217"/>
       <c r="AK308" s="217"/>
     </row>
-    <row r="309" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A309" s="65" t="s">
         <v>573</v>
       </c>
@@ -27361,7 +27375,7 @@
       <c r="AJ309" s="217"/>
       <c r="AK309" s="217"/>
     </row>
-    <row r="310" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A310" s="65" t="s">
         <v>573</v>
       </c>
@@ -27448,7 +27462,7 @@
       <c r="AJ310" s="217"/>
       <c r="AK310" s="217"/>
     </row>
-    <row r="311" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A311" s="65" t="s">
         <v>573</v>
       </c>
@@ -27535,7 +27549,7 @@
       <c r="AJ311" s="217"/>
       <c r="AK311" s="217"/>
     </row>
-    <row r="312" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A312" s="65" t="s">
         <v>573</v>
       </c>
@@ -27622,7 +27636,7 @@
       <c r="AJ312" s="217"/>
       <c r="AK312" s="217"/>
     </row>
-    <row r="313" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A313" s="65" t="s">
         <v>573</v>
       </c>
@@ -27709,7 +27723,7 @@
       <c r="AJ313" s="217"/>
       <c r="AK313" s="217"/>
     </row>
-    <row r="314" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A314" s="65" t="s">
         <v>573</v>
       </c>
@@ -27796,7 +27810,7 @@
       <c r="AJ314" s="217"/>
       <c r="AK314" s="217"/>
     </row>
-    <row r="315" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A315" s="65" t="s">
         <v>573</v>
       </c>
@@ -27883,7 +27897,7 @@
       <c r="AJ315" s="217"/>
       <c r="AK315" s="217"/>
     </row>
-    <row r="316" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A316" s="65" t="s">
         <v>573</v>
       </c>
@@ -27970,7 +27984,7 @@
       <c r="AJ316" s="217"/>
       <c r="AK316" s="217"/>
     </row>
-    <row r="317" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A317" s="65" t="s">
         <v>573</v>
       </c>
@@ -28057,7 +28071,7 @@
       <c r="AJ317" s="217"/>
       <c r="AK317" s="217"/>
     </row>
-    <row r="318" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A318" s="65" t="s">
         <v>573</v>
       </c>
@@ -28144,7 +28158,7 @@
       <c r="AJ318" s="217"/>
       <c r="AK318" s="217"/>
     </row>
-    <row r="319" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A319" s="65" t="s">
         <v>573</v>
       </c>
@@ -28295,7 +28309,7 @@
       <c r="AJ320" s="217"/>
       <c r="AK320" s="217"/>
     </row>
-    <row r="321" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A321" s="65" t="s">
         <v>573</v>
       </c>
@@ -28446,7 +28460,7 @@
       <c r="AJ322" s="217"/>
       <c r="AK322" s="217"/>
     </row>
-    <row r="323" spans="1:37" s="65" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:37" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A323" s="65" t="s">
         <v>573</v>
       </c>
@@ -28537,16 +28551,16 @@
       <c r="A324" s="178" t="s">
         <v>567</v>
       </c>
-      <c r="B324" s="247" t="s">
+      <c r="B324" s="236" t="s">
         <v>560</v>
       </c>
-      <c r="C324" s="247"/>
+      <c r="C324" s="236"/>
       <c r="D324" s="153"/>
       <c r="E324" s="153"/>
       <c r="F324" s="198"/>
       <c r="G324" s="199">
         <f>SUBTOTAL(9,G7:G323)</f>
-        <v>3710</v>
+        <v>4055561.1203199998</v>
       </c>
       <c r="Q324" s="200"/>
       <c r="R324" s="153"/>
@@ -28703,7 +28717,7 @@
       <c r="AJ327" s="219"/>
       <c r="AK327" s="219"/>
     </row>
-    <row r="328" spans="1:37" s="178" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:37" s="178" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A328" s="178" t="s">
         <v>567</v>
       </c>
@@ -28789,7 +28803,7 @@
       <c r="AJ328" s="219"/>
       <c r="AK328" s="219"/>
     </row>
-    <row r="329" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A329" s="178" t="s">
         <v>567</v>
       </c>
@@ -28964,7 +28978,7 @@
       <c r="AJ331" s="219"/>
       <c r="AK331" s="219"/>
     </row>
-    <row r="332" spans="1:37" s="178" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:37" s="178" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A332" s="178" t="s">
         <v>567</v>
       </c>
@@ -29140,7 +29154,7 @@
       <c r="AJ334" s="219"/>
       <c r="AK334" s="219"/>
     </row>
-    <row r="335" spans="1:37" s="178" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:37" s="178" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A335" s="178" t="s">
         <v>567</v>
       </c>
@@ -29226,7 +29240,7 @@
       <c r="AJ335" s="219"/>
       <c r="AK335" s="219"/>
     </row>
-    <row r="336" spans="1:37" s="178" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:37" s="178" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A336" s="178" t="s">
         <v>567</v>
       </c>
@@ -29357,7 +29371,7 @@
       <c r="AJ337" s="219"/>
       <c r="AK337" s="219"/>
     </row>
-    <row r="338" spans="1:37" s="178" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:37" s="178" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A338" s="178" t="s">
         <v>567</v>
       </c>
@@ -29443,7 +29457,7 @@
       <c r="AJ338" s="219"/>
       <c r="AK338" s="219"/>
     </row>
-    <row r="339" spans="1:37" s="178" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:37" s="178" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A339" s="178" t="s">
         <v>567</v>
       </c>
@@ -29574,7 +29588,7 @@
       <c r="AJ340" s="219"/>
       <c r="AK340" s="219"/>
     </row>
-    <row r="341" spans="1:37" s="178" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:37" s="178" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A341" s="178" t="s">
         <v>567</v>
       </c>
@@ -29660,7 +29674,7 @@
       <c r="AJ341" s="219"/>
       <c r="AK341" s="219"/>
     </row>
-    <row r="342" spans="1:37" s="178" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:37" s="178" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A342" s="178" t="s">
         <v>567</v>
       </c>
@@ -29746,7 +29760,7 @@
       <c r="AJ342" s="219"/>
       <c r="AK342" s="219"/>
     </row>
-    <row r="343" spans="1:37" s="178" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:37" s="178" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A343" s="178" t="s">
         <v>567</v>
       </c>
@@ -29877,7 +29891,7 @@
       <c r="AJ344" s="219"/>
       <c r="AK344" s="219"/>
     </row>
-    <row r="345" spans="1:37" s="178" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:37" s="178" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A345" s="178" t="s">
         <v>567</v>
       </c>
@@ -29963,7 +29977,7 @@
       <c r="AJ345" s="219"/>
       <c r="AK345" s="219"/>
     </row>
-    <row r="346" spans="1:37" hidden="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A346" s="178" t="s">
         <v>567</v>
       </c>
@@ -30048,7 +30062,7 @@
       <c r="AJ346" s="218"/>
       <c r="AK346" s="218"/>
     </row>
-    <row r="347" spans="1:37" s="178" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:37" s="178" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A347" s="178" t="s">
         <v>567</v>
       </c>
@@ -30224,7 +30238,7 @@
       <c r="AJ349" s="219"/>
       <c r="AK349" s="219"/>
     </row>
-    <row r="350" spans="1:37" s="178" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:37" s="178" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A350" s="178" t="s">
         <v>567</v>
       </c>
@@ -30355,7 +30369,7 @@
       <c r="AJ351" s="219"/>
       <c r="AK351" s="219"/>
     </row>
-    <row r="352" spans="1:37" s="178" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:37" s="178" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A352" s="178" t="s">
         <v>567</v>
       </c>
@@ -30441,7 +30455,7 @@
       <c r="AJ352" s="219"/>
       <c r="AK352" s="219"/>
     </row>
-    <row r="353" spans="1:38" s="178" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:38" s="178" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A353" s="178" t="s">
         <v>567</v>
       </c>
@@ -30534,33 +30548,33 @@
       <c r="E354" s="140"/>
       <c r="G354" s="142">
         <f>SUBTOTAL(9,G325:P353)</f>
-        <v>0</v>
+        <v>538745.4</v>
       </c>
       <c r="X354" s="177">
         <f>SUBTOTAL(9,X5:X353)</f>
-        <v>0</v>
+        <v>1206612.54</v>
       </c>
       <c r="Y354" s="177"/>
       <c r="Z354" s="177"/>
       <c r="AA354" s="177">
         <f>SUBTOTAL(9,AA5:AA353)</f>
-        <v>0</v>
+        <v>103769.64</v>
       </c>
       <c r="AB354" s="177"/>
       <c r="AC354" s="177"/>
       <c r="AD354" s="177">
         <f>SUBTOTAL(9,AD5:AD353)</f>
-        <v>0</v>
+        <v>530339.16999999993</v>
       </c>
       <c r="AE354" s="177">
         <f>SUM(AE6:AE353)</f>
-        <v>-161156.51999999996</v>
+        <v>-204873.36</v>
       </c>
       <c r="AF354" s="177"/>
       <c r="AG354" s="177"/>
       <c r="AH354" s="177">
         <f t="shared" ref="AH354:AK354" si="178">SUBTOTAL(9,AH5:AH353)</f>
-        <v>0</v>
+        <v>127542.73000000001</v>
       </c>
       <c r="AI354" s="177"/>
       <c r="AJ354" s="177"/>
@@ -30570,7 +30584,7 @@
       </c>
       <c r="AL354" s="222">
         <f>(AK354+AH354)</f>
-        <v>13880</v>
+        <v>141422.73000000001</v>
       </c>
     </row>
     <row r="355" spans="1:38" ht="21" hidden="1" x14ac:dyDescent="0.4">
@@ -30580,11 +30594,11 @@
       <c r="E355" s="140"/>
       <c r="G355" s="177">
         <f>G324-G354</f>
-        <v>3710</v>
+        <v>3516815.7203199998</v>
       </c>
       <c r="AL355" s="222">
         <f>AE354-AA354</f>
-        <v>-161156.51999999996</v>
+        <v>-308643</v>
       </c>
     </row>
     <row r="356" spans="1:38" ht="21" hidden="1" x14ac:dyDescent="0.4">
@@ -30594,22 +30608,28 @@
       <c r="E356" s="140"/>
       <c r="G356" s="142">
         <f>SUM(G6:G353)</f>
-        <v>5119348.2803200018</v>
+        <v>9171199.4006399997</v>
       </c>
       <c r="AL356" s="224">
         <f>SUM(AL354:AL355)</f>
-        <v>-147276.51999999996</v>
+        <v>-167220.26999999999</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A5:AL356" xr:uid="{9E4CE30C-FDA8-46D0-A462-CA10E19C3D2E}">
-    <filterColumn colId="0">
+    <filterColumn colId="18">
       <filters>
-        <filter val="MAYOR M"/>
+        <filter val="100.00%"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <mergeCells count="17">
+    <mergeCell ref="V2:X3"/>
+    <mergeCell ref="AF2:AH3"/>
+    <mergeCell ref="AI2:AK3"/>
+    <mergeCell ref="AB2:AD3"/>
+    <mergeCell ref="Y2:AA3"/>
+    <mergeCell ref="AE2:AE3"/>
     <mergeCell ref="B324:C324"/>
     <mergeCell ref="Q2:S3"/>
     <mergeCell ref="H3:J3"/>
@@ -30621,12 +30641,6 @@
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="F2:F4"/>
     <mergeCell ref="G2:G4"/>
-    <mergeCell ref="V2:X3"/>
-    <mergeCell ref="AF2:AH3"/>
-    <mergeCell ref="AI2:AK3"/>
-    <mergeCell ref="AB2:AD3"/>
-    <mergeCell ref="Y2:AA3"/>
-    <mergeCell ref="AE2:AE3"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="D325:F326">

</xml_diff>